<commit_message>
Finished reading value in from .xlsx file and storing as an Experiment object
</commit_message>
<xml_diff>
--- a/test_input/ynb.xlsx
+++ b/test_input/ynb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamwojciak/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamwojciak/Documents/Git/Smith Lab/Smith Lab Spreadsheet Formatter/test_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CAA372F-116F-0649-850B-10DD438F674B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A15FCD8-EF22-7A4E-BD19-FA84978F0DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16900" yWindow="660" windowWidth="21340" windowHeight="21500" xr2:uid="{2C9C3107-7256-9B4F-8FEB-8AED9DC80046}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="of_Initial_Value">'Raw Data'!$F$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,8 +71,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="\D\a\y\ 0"/>
-    <numFmt numFmtId="174" formatCode="&quot;Day &quot;0"/>
+    <numFmt numFmtId="164" formatCode="\D\a\y\ 0"/>
+    <numFmt numFmtId="165" formatCode="&quot;Day &quot;0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -152,35 +152,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,752 +519,659 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686FCE2-11E3-514C-8CE6-EBB6F3EC5367}">
-  <dimension ref="A1:AD38"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="14">
         <v>4</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="5">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15">
         <v>7</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="3">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14">
         <v>14</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="5">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15">
         <v>18</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="3">
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="14">
         <v>28</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="5">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="15">
         <v>31</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6" t="s">
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
         <f>PRODUCT(D3, E3)</f>
         <v>234</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="1">
         <v>234</v>
       </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <f>(D3*E3)/C3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="3">
         <v>293</v>
       </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="16">
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
         <f>(G3*H3)/C3</f>
         <v>1.2521367521367521</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="1">
         <v>245</v>
       </c>
-      <c r="K3" s="6">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9">
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
         <f>(J3*K3)/C3</f>
         <v>1.0470085470085471</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="3">
         <v>133</v>
       </c>
-      <c r="N3" s="7">
-        <v>1</v>
-      </c>
-      <c r="O3" s="10">
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
         <f>(M3*N3)/C3</f>
         <v>0.56837606837606836</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="1">
         <v>32</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="1">
         <v>0.1</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="4">
         <f>(P3*Q3)/C3</f>
         <v>1.3675213675213675E-2</v>
       </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="10">
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="5">
         <f>(S3*T3)/C3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="13">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="2">
         <f t="shared" ref="C4:C10" si="0">PRODUCT(D4, E4)</f>
         <v>205</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="1">
         <v>205</v>
       </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
         <f t="shared" ref="F4:F10" si="1">(D4*E4)/C4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="3">
         <v>304</v>
       </c>
-      <c r="H4" s="17">
-        <v>1</v>
-      </c>
-      <c r="I4" s="16">
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
         <f t="shared" ref="I4:I10" si="2">(G4*H4)/C4</f>
         <v>1.4829268292682927</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="1">
         <v>215</v>
       </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="9">
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
         <f t="shared" ref="L4:L10" si="3">(J4*K4)/C4</f>
         <v>1.0487804878048781</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="3">
         <v>107</v>
       </c>
-      <c r="N4" s="7">
-        <v>1</v>
-      </c>
-      <c r="O4" s="10">
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5">
         <f t="shared" ref="O4:O10" si="4">(M4*N4)/C4</f>
         <v>0.52195121951219514</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="1">
         <v>79</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="1">
         <v>0.1</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="4">
         <f t="shared" ref="R4:R10" si="5">(P4*Q4)/C4</f>
         <v>3.8536585365853658E-2</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="10">
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="5">
         <f t="shared" ref="U4:U10" si="6">(S4*T4)/C4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
-      <c r="B5" s="13">
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>214</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>214</v>
       </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="3">
         <v>209</v>
       </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="16">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
         <f t="shared" si="2"/>
         <v>0.97663551401869164</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="1">
         <v>176</v>
       </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="9">
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
         <f t="shared" si="3"/>
         <v>0.82242990654205606</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="3">
         <v>49</v>
       </c>
-      <c r="N5" s="7">
-        <v>1</v>
-      </c>
-      <c r="O5" s="10">
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5">
         <f t="shared" si="4"/>
         <v>0.22897196261682243</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="1">
         <v>94</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="1">
         <v>0.1</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="4">
         <f t="shared" si="5"/>
         <v>4.3925233644859812E-2</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="10">
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
-      <c r="B6" s="13">
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="1">
         <v>216</v>
       </c>
-      <c r="E6" s="6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="3">
         <v>263</v>
       </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="16">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
         <f t="shared" si="2"/>
         <v>1.2175925925925926</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="1">
         <v>194</v>
       </c>
-      <c r="K6" s="6">
-        <v>1</v>
-      </c>
-      <c r="L6" s="9">
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" si="3"/>
         <v>0.89814814814814814</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="3">
         <v>51</v>
       </c>
-      <c r="N6" s="7">
-        <v>1</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="5">
         <f t="shared" si="4"/>
         <v>0.2361111111111111</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="1">
         <v>71</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="1">
         <v>0.1</v>
       </c>
-      <c r="R6" s="9">
+      <c r="R6" s="4">
         <f t="shared" si="5"/>
         <v>3.2870370370370376E-2</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="10">
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="1">
         <v>250</v>
       </c>
-      <c r="E7" s="6">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="3">
         <v>228</v>
       </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="16">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
         <f t="shared" si="2"/>
         <v>0.91200000000000003</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="1">
         <v>195</v>
       </c>
-      <c r="K7" s="6">
-        <v>1</v>
-      </c>
-      <c r="L7" s="9">
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="3"/>
         <v>0.78</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="3">
         <v>97</v>
       </c>
-      <c r="N7" s="7">
-        <v>1</v>
-      </c>
-      <c r="O7" s="10">
+      <c r="N7" s="3">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5">
         <f t="shared" si="4"/>
         <v>0.38800000000000001</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="1">
         <v>38</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="1">
         <v>0.1</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7" s="4">
         <f t="shared" si="5"/>
         <v>1.5200000000000002E-2</v>
       </c>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="10">
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>285</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="1">
         <v>285</v>
       </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="3">
         <v>296</v>
       </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="16">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
         <f t="shared" si="2"/>
         <v>1.0385964912280701</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="1">
         <v>158</v>
       </c>
-      <c r="K8" s="6">
-        <v>1</v>
-      </c>
-      <c r="L8" s="9">
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="3"/>
         <v>0.55438596491228065</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="3">
         <v>54</v>
       </c>
-      <c r="N8" s="7">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10">
+      <c r="N8" s="3">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
         <f t="shared" si="4"/>
         <v>0.18947368421052632</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="1">
         <v>93</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="1">
         <v>0.1</v>
       </c>
-      <c r="R8" s="9">
+      <c r="R8" s="4">
         <f t="shared" si="5"/>
         <v>3.2631578947368421E-2</v>
       </c>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="10">
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>212</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="1">
         <v>212</v>
       </c>
-      <c r="E9" s="6">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="3">
         <v>275</v>
       </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16">
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
         <f t="shared" si="2"/>
         <v>1.2971698113207548</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="1">
         <v>179</v>
       </c>
-      <c r="K9" s="6">
-        <v>1</v>
-      </c>
-      <c r="L9" s="9">
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
         <f t="shared" si="3"/>
         <v>0.84433962264150941</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="3">
         <v>95</v>
       </c>
-      <c r="N9" s="7">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10">
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
         <f t="shared" si="4"/>
         <v>0.44811320754716982</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="1">
         <v>43</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="1">
         <v>0.1</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9" s="4">
         <f t="shared" si="5"/>
         <v>2.0283018867924527E-2</v>
       </c>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="10">
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>279</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="1">
         <v>279</v>
       </c>
-      <c r="E10" s="6">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="3">
         <v>299</v>
       </c>
-      <c r="H10" s="7">
-        <v>1</v>
-      </c>
-      <c r="I10" s="16">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
         <f t="shared" si="2"/>
         <v>1.0716845878136201</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="1">
         <v>167</v>
       </c>
-      <c r="K10" s="6">
-        <v>1</v>
-      </c>
-      <c r="L10" s="9">
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
         <f t="shared" si="3"/>
         <v>0.59856630824372759</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="3">
         <v>80</v>
       </c>
-      <c r="N10" s="7">
-        <v>1</v>
-      </c>
-      <c r="O10" s="10">
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5">
         <f t="shared" si="4"/>
         <v>0.28673835125448027</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="1">
         <v>94</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="1">
         <v>0.1</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="4">
         <f t="shared" si="5"/>
         <v>3.3691756272401438E-2</v>
       </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="10">
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1285,22 +1191,22 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="10">
         <v>4</v>
       </c>
-      <c r="C1" s="18">
+      <c r="C1" s="10">
         <v>7</v>
       </c>
-      <c r="D1" s="18">
+      <c r="D1" s="10">
         <v>14</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="10">
         <v>18</v>
       </c>
-      <c r="F1" s="18">
+      <c r="F1" s="10">
         <v>28</v>
       </c>
-      <c r="G1" s="18">
+      <c r="G1" s="10">
         <v>31</v>
       </c>
     </row>
@@ -1308,27 +1214,27 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="11">
         <f>'Raw Data'!F3</f>
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="11">
         <f>'Raw Data'!I3</f>
         <v>1.2521367521367521</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="11">
         <f>'Raw Data'!L3</f>
         <v>1.0470085470085471</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="11">
         <f>'Raw Data'!O3</f>
         <v>0.56837606837606836</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="11">
         <f>'Raw Data'!R3</f>
         <v>1.3675213675213675E-2</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="11">
         <f>'Raw Data'!U3</f>
         <v>0</v>
       </c>
@@ -1337,27 +1243,27 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="11">
         <f>'Raw Data'!F4</f>
         <v>1</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="11">
         <f>'Raw Data'!I4</f>
         <v>1.4829268292682927</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="11">
         <f>'Raw Data'!L4</f>
         <v>1.0487804878048781</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="11">
         <f>'Raw Data'!O4</f>
         <v>0.52195121951219514</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="11">
         <f>'Raw Data'!R4</f>
         <v>3.8536585365853658E-2</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="11">
         <f>'Raw Data'!U4</f>
         <v>0</v>
       </c>
@@ -1366,27 +1272,27 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="11">
         <f>'Raw Data'!F5</f>
         <v>1</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="11">
         <f>'Raw Data'!I5</f>
         <v>0.97663551401869164</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="11">
         <f>'Raw Data'!L5</f>
         <v>0.82242990654205606</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="11">
         <f>'Raw Data'!O5</f>
         <v>0.22897196261682243</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="11">
         <f>'Raw Data'!R5</f>
         <v>4.3925233644859812E-2</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="11">
         <f>'Raw Data'!U5</f>
         <v>0</v>
       </c>
@@ -1395,27 +1301,27 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="11">
         <f>'Raw Data'!F6</f>
         <v>1</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="11">
         <f>'Raw Data'!I6</f>
         <v>1.2175925925925926</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="11">
         <f>'Raw Data'!L6</f>
         <v>0.89814814814814814</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="11">
         <f>'Raw Data'!O6</f>
         <v>0.2361111111111111</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="11">
         <f>'Raw Data'!R6</f>
         <v>3.2870370370370376E-2</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="11">
         <f>'Raw Data'!U6</f>
         <v>0</v>
       </c>
@@ -1424,27 +1330,27 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="11">
         <f>'Raw Data'!F7</f>
         <v>1</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="11">
         <f>'Raw Data'!I7</f>
         <v>0.91200000000000003</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="11">
         <f>'Raw Data'!L7</f>
         <v>0.78</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="11">
         <f>'Raw Data'!O7</f>
         <v>0.38800000000000001</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="11">
         <f>'Raw Data'!R7</f>
         <v>1.5200000000000002E-2</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="11">
         <f>'Raw Data'!U7</f>
         <v>0</v>
       </c>
@@ -1453,27 +1359,27 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="11">
         <f>'Raw Data'!F8</f>
         <v>1</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="11">
         <f>'Raw Data'!I8</f>
         <v>1.0385964912280701</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="11">
         <f>'Raw Data'!L8</f>
         <v>0.55438596491228065</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="11">
         <f>'Raw Data'!O8</f>
         <v>0.18947368421052632</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="11">
         <f>'Raw Data'!R8</f>
         <v>3.2631578947368421E-2</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="11">
         <f>'Raw Data'!U8</f>
         <v>0</v>
       </c>
@@ -1482,27 +1388,27 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="11">
         <f>'Raw Data'!F9</f>
         <v>1</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="11">
         <f>'Raw Data'!I9</f>
         <v>1.2971698113207548</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="11">
         <f>'Raw Data'!L9</f>
         <v>0.84433962264150941</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="11">
         <f>'Raw Data'!O9</f>
         <v>0.44811320754716982</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="11">
         <f>'Raw Data'!R9</f>
         <v>2.0283018867924527E-2</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="11">
         <f>'Raw Data'!U9</f>
         <v>0</v>
       </c>
@@ -1511,27 +1417,27 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="11">
         <f>'Raw Data'!F10</f>
         <v>1</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="11">
         <f>'Raw Data'!I10</f>
         <v>1.0716845878136201</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="11">
         <f>'Raw Data'!L10</f>
         <v>0.59856630824372759</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="11">
         <f>'Raw Data'!O10</f>
         <v>0.28673835125448027</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="11">
         <f>'Raw Data'!R10</f>
         <v>3.3691756272401438E-2</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="11">
         <f>'Raw Data'!U10</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Wrote code to output first part of other output
</commit_message>
<xml_diff>
--- a/test_input/ynb.xlsx
+++ b/test_input/ynb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamwojciak/Documents/Git/Smith Lab/Smith Lab Spreadsheet Formatter/test_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A15FCD8-EF22-7A4E-BD19-FA84978F0DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DC7308-FEF0-4D41-B90D-1837F11021CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16900" yWindow="660" windowWidth="21340" windowHeight="21500" xr2:uid="{2C9C3107-7256-9B4F-8FEB-8AED9DC80046}"/>
   </bookViews>
@@ -152,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -165,21 +165,24 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,56 +525,56 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="G1" sqref="G1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>4</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="19">
         <v>7</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="14">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="13">
         <v>14</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="15">
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="12">
         <v>18</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="14">
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13">
         <v>28</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="12">
         <v>31</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
@@ -628,7 +631,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6">
@@ -696,7 +699,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -762,7 +765,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -828,7 +831,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -894,7 +897,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7">
@@ -962,7 +965,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -1028,7 +1031,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -1094,7 +1097,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -1161,17 +1164,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>